<commit_message>
Augmented_datasets upload and graph_visualization
</commit_message>
<xml_diff>
--- a/data/badge_dataset_updated.xlsx
+++ b/data/badge_dataset_updated.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Badgelens\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CEED92-2886-40CF-A286-EEABA0E44D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>badge_id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>issuer</t>
   </si>
   <si>
@@ -185,17 +188,63 @@
   </si>
   <si>
     <t>Advanced</t>
+  </si>
+  <si>
+    <t>badge_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coursera: Intro to Python &amp; data analysis. Beginner.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DataCamp: Learn Pandas &amp; SQL basics. Intermediate.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Udacity: ML fundamentals with Python. Intermediate.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DeepLearning.AI: Advanced neural nets &amp; TensorFlow. Advanced.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI Policy: Overview of ethics &amp; policy in AI. Advanced.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWS: Intro to cloud computing. Beginner.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Udacity: Basics of DevOps with Kubernetes &amp; CI/CD. Intermediate.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>edX: Fundamentals of cybersecurity &amp; networking. Beginner.</t>
+  </si>
+  <si>
+    <t>Offensive Security: Advanced ethical hacking techniques. Advanced.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Google: Core UI/UX design fundamentals. Beginner.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,8 +252,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -250,17 +306,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +362,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -332,6 +396,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -366,9 +431,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,234 +607,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="31.125" customWidth="1"/>
+    <col min="6" max="6" width="16.75" customWidth="1"/>
+    <col min="7" max="7" width="60.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="G3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>48</v>
       </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>53</v>
       </c>
-      <c r="F11" t="s">
-        <v>54</v>
+      <c r="G11" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>